<commit_message>
Fix issues DURM-327 & DURM-328
</commit_message>
<xml_diff>
--- a/data/reporting/end_user_to_bb_job_role_report_qualification.xlsx
+++ b/data/reporting/end_user_to_bb_job_role_report_qualification.xlsx
@@ -15,7 +15,7 @@
     <externalReference r:id="rId4"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'EUDL to Backbone Qualification'!$A$3:$BF$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'EUDL to Backbone Qualification'!$A$3:$BG$3</definedName>
     <definedName name="Directors">[1]Definitions!$B$75:$C$96</definedName>
     <definedName name="HML">[2]Data!$B$2:$B$4</definedName>
     <definedName name="Org">[2]Data!$C$2:$C$22</definedName>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>Role Mapping New Deployment Template</t>
   </si>
@@ -204,6 +204,9 @@
   </si>
   <si>
     <t>Backbone Job Roles</t>
+  </si>
+  <si>
+    <t>Mapping Type</t>
   </si>
 </sst>
 </file>
@@ -1155,10 +1158,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BG3"/>
+  <dimension ref="A1:BH3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="23" ySplit="3" topLeftCell="BG4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="24" ySplit="3" topLeftCell="Y4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="W1" sqref="W1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
       <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
@@ -1174,15 +1177,15 @@
     <col min="15" max="15" width="7.85546875" style="8" collapsed="1"/>
     <col min="16" max="18" width="7.85546875" style="8"/>
     <col min="19" max="19" width="7.85546875" style="8" collapsed="1"/>
-    <col min="20" max="21" width="0" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="20" max="21" width="7.85546875" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="22" max="22" width="7.85546875" style="8" collapsed="1"/>
-    <col min="23" max="23" width="7.85546875" style="8"/>
-    <col min="24" max="58" width="0" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="59" max="59" width="7.85546875" style="8" collapsed="1"/>
-    <col min="60" max="16384" width="7.85546875" style="8"/>
+    <col min="23" max="24" width="7.85546875" style="8"/>
+    <col min="25" max="59" width="0" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="60" max="60" width="7.85546875" style="8" collapsed="1"/>
+    <col min="61" max="16384" width="7.85546875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" s="9" customFormat="1" ht="6" customHeight="1">
+    <row r="1" spans="1:59" s="9" customFormat="1" ht="6" customHeight="1">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -1203,7 +1206,7 @@
       <c r="P1" s="13"/>
       <c r="Q1" s="13"/>
     </row>
-    <row r="2" spans="1:58" s="12" customFormat="1" ht="162.75" customHeight="1" thickBot="1">
+    <row r="2" spans="1:59" s="12" customFormat="1" ht="162.75" customHeight="1" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1273,113 +1276,116 @@
       <c r="W2" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="X2" s="11" t="s">
+      <c r="X2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y2" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="Y2" s="11" t="s">
+      <c r="Z2" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="Z2" s="11" t="s">
+      <c r="AA2" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="AA2" s="11" t="s">
+      <c r="AB2" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="AB2" s="11" t="s">
+      <c r="AC2" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="AC2" s="11" t="s">
+      <c r="AD2" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="AD2" s="11" t="s">
+      <c r="AE2" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="AE2" s="11" t="s">
+      <c r="AF2" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="AF2" s="11" t="s">
+      <c r="AG2" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AG2" s="11" t="s">
+      <c r="AH2" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="AH2" s="11" t="s">
+      <c r="AI2" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="AI2" s="11" t="s">
+      <c r="AJ2" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="AJ2" s="11" t="s">
+      <c r="AK2" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="AK2" s="11" t="s">
+      <c r="AL2" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="AL2" s="11" t="s">
+      <c r="AM2" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="AM2" s="11" t="s">
+      <c r="AN2" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="AN2" s="11" t="s">
+      <c r="AO2" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="AO2" s="11" t="s">
+      <c r="AP2" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="AP2" s="11" t="s">
+      <c r="AQ2" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="AQ2" s="11" t="s">
+      <c r="AR2" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="AR2" s="11" t="s">
+      <c r="AS2" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="AS2" s="11" t="s">
+      <c r="AT2" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="AT2" s="11" t="s">
+      <c r="AU2" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="AU2" s="11" t="s">
+      <c r="AV2" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="AV2" s="11" t="s">
+      <c r="AW2" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="AW2" s="11" t="s">
+      <c r="AX2" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="AX2" s="11" t="s">
+      <c r="AY2" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="AY2" s="11" t="s">
+      <c r="AZ2" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="AZ2" s="11" t="s">
+      <c r="BA2" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="BA2" s="11" t="s">
+      <c r="BB2" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="BB2" s="11" t="s">
+      <c r="BC2" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="BC2" s="11" t="s">
+      <c r="BD2" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="BD2" s="11" t="s">
+      <c r="BE2" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="BE2" s="11" t="s">
+      <c r="BF2" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="BF2" s="11" t="s">
+      <c r="BG2" s="11" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:58" s="2" customFormat="1" ht="16.5" thickBot="1">
+    <row r="3" spans="1:59" s="2" customFormat="1" ht="16.5" thickBot="1">
       <c r="A3" s="3"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -1438,9 +1444,10 @@
       <c r="BD3" s="7"/>
       <c r="BE3" s="7"/>
       <c r="BF3" s="7"/>
+      <c r="BG3" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="A3:BF3"/>
+  <autoFilter ref="A3:BG3"/>
   <mergeCells count="1">
     <mergeCell ref="A1:Q1"/>
   </mergeCells>

</xml_diff>